<commit_message>
Updated planning (added urenschatting)
</commit_message>
<xml_diff>
--- a/Documenten/Planning.xlsx
+++ b/Documenten/Planning.xlsx
@@ -24,20 +24,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="35">
   <si>
     <t>Taak</t>
   </si>
   <si>
-    <t>Deadline</t>
-  </si>
-  <si>
     <t>UI bouwen</t>
   </si>
   <si>
-    <t>Architectuur</t>
-  </si>
-  <si>
     <t>Simpuls overleg</t>
   </si>
   <si>
@@ -71,9 +65,6 @@
     <t>Stephan, Franck, Jasper</t>
   </si>
   <si>
-    <t>Steffan, Stephan, Jasper</t>
-  </si>
-  <si>
     <t>Steffan</t>
   </si>
   <si>
@@ -89,9 +80,6 @@
     <t>Moet nog gebeuren</t>
   </si>
   <si>
-    <t>Brian, Xander</t>
-  </si>
-  <si>
     <t>Playtesten</t>
   </si>
   <si>
@@ -102,13 +90,52 @@
   </si>
   <si>
     <t>_</t>
+  </si>
+  <si>
+    <t>Ureninschatting</t>
+  </si>
+  <si>
+    <t>2uur</t>
+  </si>
+  <si>
+    <t>3uur</t>
+  </si>
+  <si>
+    <t>Daadwerkelijke uren</t>
+  </si>
+  <si>
+    <t>1uur tot nu toe</t>
+  </si>
+  <si>
+    <t>Steffan, Stephan, Jasper, Xander Brian</t>
+  </si>
+  <si>
+    <t>5uur</t>
+  </si>
+  <si>
+    <t>10uur</t>
+  </si>
+  <si>
+    <t>6uur tot nu toe</t>
+  </si>
+  <si>
+    <t>20uur</t>
+  </si>
+  <si>
+    <t>80uur</t>
+  </si>
+  <si>
+    <t>1uur</t>
+  </si>
+  <si>
+    <t>3uur tot nu toe</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -141,6 +168,14 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -198,22 +233,27 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="4"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="5" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="6">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
+    <cellStyle name="Explanatory Text" xfId="5" builtinId="53"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -495,18 +535,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V12"/>
+  <dimension ref="A1:V11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="36.7109375" customWidth="1"/>
-    <col min="2" max="2" width="28" customWidth="1"/>
+    <col min="1" max="2" width="36.7109375" customWidth="1"/>
     <col min="3" max="3" width="18.5703125" customWidth="1"/>
     <col min="4" max="4" width="15.28515625" customWidth="1"/>
+    <col min="5" max="5" width="19.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.25">
@@ -514,15 +554,17 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="1"/>
+        <v>22</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>25</v>
+      </c>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
@@ -543,124 +585,163 @@
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>20</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E3" s="5"/>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>11</v>
       </c>
+      <c r="D4" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>13</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E5" s="5"/>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>20</v>
+        <v>15</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="B7" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>17</v>
+        <v>14</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>17</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E8" s="5"/>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="B10" t="s">
-        <v>15</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>11</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E10" s="5"/>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B11" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>23</v>
-      </c>
-      <c r="B12" t="s">
-        <v>25</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>20</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>